<commit_message>
ODK-X and helper app init.
</commit_message>
<xml_diff>
--- a/odk_app/config/assets/framework/framework.xlsx
+++ b/odk_app/config/assets/framework/framework.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Joey\Desktop\dev\classes\capstone\app-designer-2.1.6\app\config\assets\framework\forms\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Joey\Desktop\dev\classes\capstone\app-designer-2.1.6\app\config\assets\framework\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02652925-DFF4-45F0-B670-05608A199DAC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6650D00-9D41-42B8-8BA5-B05B3CF060D2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="330" windowWidth="29040" windowHeight="15990" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="330" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="initial" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="158">
   <si>
     <t>clause</t>
   </si>
@@ -491,6 +491,30 @@
   </si>
   <si>
     <t>'?' + odkSurvey.getHashString('life_check')</t>
+  </si>
+  <si>
+    <t>ingrowth</t>
+  </si>
+  <si>
+    <t>Tree Ingrowth Form</t>
+  </si>
+  <si>
+    <t>mortality</t>
+  </si>
+  <si>
+    <t>'?' + odkSurvey.getHashString('mortality')</t>
+  </si>
+  <si>
+    <t>'?' + odkSurvey.getHashString('ingrowth')</t>
+  </si>
+  <si>
+    <t>Open tree mortality form</t>
+  </si>
+  <si>
+    <t>Open tree ingrowth form</t>
+  </si>
+  <si>
+    <t>Tree Mortality Form</t>
   </si>
 </sst>
 </file>
@@ -509,6 +533,7 @@
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -836,7 +861,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -1412,10 +1437,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AEB3E646-09D4-42BF-884F-866C24A046CD}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1447,6 +1472,28 @@
         <v>131</v>
       </c>
     </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>129</v>
+      </c>
+      <c r="B3" t="s">
+        <v>150</v>
+      </c>
+      <c r="C3" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>129</v>
+      </c>
+      <c r="B4" t="s">
+        <v>152</v>
+      </c>
+      <c r="C4" t="s">
+        <v>157</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1454,20 +1501,21 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7603C5B8-5522-4D8D-A129-D36D49614447}">
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:G16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="38.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="49.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -1556,6 +1604,48 @@
         <v>146</v>
       </c>
     </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B12" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="E12" t="s">
+        <v>147</v>
+      </c>
+      <c r="G12" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C13" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B15" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="E15" t="s">
+        <v>147</v>
+      </c>
+      <c r="G15" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C16" t="s">
+        <v>146</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>